<commit_message>
Bollinger bands functions (bb percentage, bb width and normal bb) added to the website
</commit_message>
<xml_diff>
--- a/sectorStocks.xlsx
+++ b/sectorStocks.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>stocks</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>LCSW</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>sf</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1340,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1349,6 +1355,22 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>